<commit_message>
Updated batch documentation and distribution
</commit_message>
<xml_diff>
--- a/doc/Manual/Batchmode/StageStructFile.xlsx
+++ b/doc/Manual/Batchmode/StageStructFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter_v2_0\doc\Manual\Batchmode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\RangeShifter2\doc\Manual\Batchmode\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -70,7 +70,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="70">
   <si>
     <t>PRep</t>
   </si>
@@ -411,9 +411,6 @@
     <t>Name of the survival stage weights matrix file (*.txt)</t>
   </si>
   <si>
-    <t>Stage-specific density-dependence in fecuntity: 0 = No, 1  = Yes</t>
-  </si>
-  <si>
     <t>Density-dependent survival coefficient</t>
   </si>
   <si>
@@ -426,15 +423,6 @@
     <t>Density-dependence in fecundity: 0 = No, 1 = Yes</t>
   </si>
   <si>
-    <t>Required if FecStageDep is 1</t>
-  </si>
-  <si>
-    <t>Required if DevStageDep is 1</t>
-  </si>
-  <si>
-    <t>Required if SurvStageDep is 1</t>
-  </si>
-  <si>
     <t>Must match simulation numbers in ParametersFile</t>
   </si>
   <si>
@@ -454,6 +442,24 @@
   </si>
   <si>
     <t>Must be &gt; 0 if SurvDensDep is 1</t>
+  </si>
+  <si>
+    <t>Stage-weighted density-dependence in fecuntity: 0 = No, 1  = Yes</t>
+  </si>
+  <si>
+    <t>Stage-weighted density-dependence in development: 0 = No, 1  = Yes</t>
+  </si>
+  <si>
+    <t>Stage-weighted density-dependence in survival: 0 = No, 1  = Yes</t>
+  </si>
+  <si>
+    <t>Required if FecStageDep is 1, otherwise NULL</t>
+  </si>
+  <si>
+    <t>Required if DevStageDep is 1, otherwise NULL</t>
+  </si>
+  <si>
+    <t>Required if SurvStageDep is 1, otherwise NULL</t>
   </si>
 </sst>
 </file>
@@ -1014,21 +1020,21 @@
         <v>48</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="D3" s="14" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1051,7 +1057,7 @@
         <v>45</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="D5" s="14"/>
     </row>
@@ -1099,7 +1105,7 @@
         <v>45</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="D9" s="14"/>
     </row>
@@ -1111,7 +1117,7 @@
         <v>45</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>53</v>
+        <v>64</v>
       </c>
       <c r="D10" s="15"/>
     </row>
@@ -1126,7 +1132,7 @@
         <v>50</v>
       </c>
       <c r="D11" s="15" t="s">
-        <v>58</v>
+        <v>67</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
@@ -1137,7 +1143,7 @@
         <v>45</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D12" s="14"/>
     </row>
@@ -1152,7 +1158,7 @@
         <v>5</v>
       </c>
       <c r="D13" s="15" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
@@ -1163,7 +1169,7 @@
         <v>45</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>53</v>
+        <v>65</v>
       </c>
       <c r="D14" s="15"/>
     </row>
@@ -1178,7 +1184,7 @@
         <v>51</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>59</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1189,7 +1195,7 @@
         <v>45</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="D16" s="14"/>
     </row>
@@ -1201,10 +1207,10 @@
         <v>43</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="D17" s="15" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1215,7 +1221,7 @@
         <v>45</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>53</v>
+        <v>66</v>
       </c>
       <c r="D18" s="15"/>
     </row>
@@ -1230,7 +1236,7 @@
         <v>52</v>
       </c>
       <c r="D19" s="15" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -1278,7 +1284,7 @@
         <v>12</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>0</v>

</xml_diff>